<commit_message>
feat(excel2json): create enabled license array in json with excel (DEV-4865) (#1697)
</commit_message>
<xml_diff>
--- a/docs/assets/data_model_templates/json_header.xlsx
+++ b/docs/assets/data_model_templates/json_header.xlsx
@@ -5,19 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noraammann/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noraammann/Documents/Cloned_GitHub/dsp-tools/docs/assets/data_model_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1587E9A-7A45-E14C-A520-49BA842A7F6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B424540-C5A4-6E49-B76B-DCCFBB8F096D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="21880" windowWidth="25540" windowHeight="9000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30520" yWindow="5040" windowWidth="29860" windowHeight="20940" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prefixes" sheetId="1" r:id="rId1"/>
     <sheet name="Project" sheetId="2" r:id="rId2"/>
     <sheet name="Description" sheetId="3" r:id="rId3"/>
     <sheet name="Keywords" sheetId="4" r:id="rId4"/>
-    <sheet name="Users" sheetId="5" r:id="rId5"/>
+    <sheet name="Licenses" sheetId="6" r:id="rId5"/>
+    <sheet name="Users" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="74">
   <si>
     <t>prefixes</t>
   </si>
@@ -224,6 +225,36 @@
   </si>
   <si>
     <t>Liddell</t>
+  </si>
+  <si>
+    <t>enabled</t>
+  </si>
+  <si>
+    <t>http://rdfh.ch/licenses/cc-by-4.0</t>
+  </si>
+  <si>
+    <t>http://rdfh.ch/licenses/cc-by-sa-4.0</t>
+  </si>
+  <si>
+    <t>http://rdfh.ch/licenses/cc-by-nc-4.0</t>
+  </si>
+  <si>
+    <t>http://rdfh.ch/licenses/cc-by-nc-sa-4.0</t>
+  </si>
+  <si>
+    <t>http://rdfh.ch/licenses/cc-by-nd-4.0</t>
+  </si>
+  <si>
+    <t>http://rdfh.ch/licenses/cc-by-nc-nd-4.0</t>
+  </si>
+  <si>
+    <t>http://rdfh.ch/licenses/ai-generated</t>
+  </si>
+  <si>
+    <t>http://rdfh.ch/licenses/unknown</t>
+  </si>
+  <si>
+    <t>http://rdfh.ch/licenses/public-domain</t>
   </si>
 </sst>
 </file>
@@ -14834,10 +14865,79 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BB52730-9A73-244A-A9DD-3B20C813D65B}">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0">
+    <sheetView zoomScale="119" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat(create)!: disallow creation of SystemAdmin (DEV-5009) (#1787)
</commit_message>
<xml_diff>
--- a/docs/assets/data_model_templates/json_header.xlsx
+++ b/docs/assets/data_model_templates/json_header.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noraammann/Documents/Cloned_GitHub/dsp-tools/docs/assets/data_model_templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nussbaum/Desktop/Cloned_GitHub_repos/dsp-tools/docs/assets/data_model_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B424540-C5A4-6E49-B76B-DCCFBB8F096D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE9246F-C1A1-BA4F-AD29-394F17F9BE01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30520" yWindow="5040" windowWidth="29860" windowHeight="20940" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prefixes" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,19 @@
     <sheet name="Licenses" sheetId="6" r:id="rId5"/>
     <sheet name="Users" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="eXIUItnczbsgwU2bhTxsCIaPyk1rdouaLJcS/mum0so="/>
     </ext>
@@ -30,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="73">
   <si>
     <t>prefixes</t>
   </si>
@@ -216,9 +227,6 @@
   </si>
   <si>
     <t>fr</t>
-  </si>
-  <si>
-    <t>systemadmin</t>
   </si>
   <si>
     <t>Alice Pleasance</t>
@@ -14868,7 +14876,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BB52730-9A73-244A-A9DD-3B20C813D65B}">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
+    <sheetView zoomScale="113" workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -14880,52 +14888,52 @@
   <sheetData>
     <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -14937,8 +14945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView zoomScale="119" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -15002,10 +15010,10 @@
         <v>45</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>47</v>
@@ -15060,7 +15068,7 @@
         <v>60</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>